<commit_message>
add excel/csv for assignment
</commit_message>
<xml_diff>
--- a/src/main/webapp/templates/questionSample.xlsx
+++ b/src/main/webapp/templates/questionSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FPTU\OJT\HANKYO\Hankyo\src\main\webapp\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9194689B-5D16-41AA-B2CD-4DD5499E9AA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72453980-A5E6-4DFD-BE88-011A05E193D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F27F130A-43A7-458D-BBB6-2531E5D7CF70}"/>
   </bookViews>
@@ -228,14 +228,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0EFB1B-BBD7-46BD-9CB2-EDD0AEE471EB}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,8 +568,11 @@
     <col min="3" max="3" width="16.109375" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1"/>
-    <col min="10" max="11" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="12.77734375" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -586,29 +594,29 @@
       <c r="F1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>34</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>36</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,29 +631,29 @@
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="4">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="4">
         <v>0</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="4">
         <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,29 +668,29 @@
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="4">
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="4">
         <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,29 +705,29 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="4">
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="4">
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="4">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,36 +735,36 @@
         <v>16</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="4">
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="4">
         <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,29 +779,30 @@
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="4">
         <v>0</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="4">
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>